<commit_message>
Risk Score related changes
</commit_message>
<xml_diff>
--- a/ReadDataFromExcelFile/src/main/resources/templates/DataSheet.xlsx
+++ b/ReadDataFromExcelFile/src/main/resources/templates/DataSheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vinod\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Workspace_Barclays\Excel-Uplad\ReadDataFromExcelFile\src\main\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="50">
   <si>
     <t>Sr.No</t>
   </si>
@@ -171,6 +171,9 @@
   </si>
   <si>
     <t>V20</t>
+  </si>
+  <si>
+    <t>External</t>
   </si>
 </sst>
 </file>
@@ -503,7 +506,7 @@
   <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="N18" activeCellId="1" sqref="N17 N18"/>
+      <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -601,6 +604,12 @@
         <v>22</v>
       </c>
       <c r="K2" s="2"/>
+      <c r="L2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M2" t="s">
+        <v>24</v>
+      </c>
       <c r="N2" t="s">
         <v>21</v>
       </c>
@@ -683,6 +692,12 @@
         <v>22</v>
       </c>
       <c r="K4" s="2"/>
+      <c r="L4" t="s">
+        <v>24</v>
+      </c>
+      <c r="M4" t="s">
+        <v>24</v>
+      </c>
       <c r="N4" t="s">
         <v>22</v>
       </c>
@@ -725,10 +740,10 @@
         <v>43913</v>
       </c>
       <c r="L5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N5" t="s">
         <v>21</v>
@@ -817,7 +832,10 @@
       </c>
       <c r="K7" s="2"/>
       <c r="L7" t="s">
-        <v>24</v>
+        <v>23</v>
+      </c>
+      <c r="M7" t="s">
+        <v>23</v>
       </c>
       <c r="N7" t="s">
         <v>21</v>
@@ -908,10 +926,10 @@
         <v>43907</v>
       </c>
       <c r="L9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N9" t="s">
         <v>21</v>
@@ -948,6 +966,12 @@
         <v>22</v>
       </c>
       <c r="K10" s="2"/>
+      <c r="L10" t="s">
+        <v>24</v>
+      </c>
+      <c r="M10" t="s">
+        <v>24</v>
+      </c>
       <c r="N10" t="s">
         <v>22</v>
       </c>
@@ -990,10 +1014,10 @@
         <v>43905</v>
       </c>
       <c r="L11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N11" t="s">
         <v>21</v>
@@ -1082,7 +1106,10 @@
       </c>
       <c r="K13" s="2"/>
       <c r="L13" t="s">
-        <v>24</v>
+        <v>23</v>
+      </c>
+      <c r="M13" t="s">
+        <v>23</v>
       </c>
       <c r="N13" t="s">
         <v>21</v>
@@ -1102,7 +1129,7 @@
         <v>31</v>
       </c>
       <c r="D14" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="E14" t="s">
         <v>32</v>
@@ -1149,7 +1176,7 @@
         <v>31</v>
       </c>
       <c r="D15" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="E15" t="s">
         <v>20</v>
@@ -1196,7 +1223,7 @@
         <v>31</v>
       </c>
       <c r="D16" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="E16" t="s">
         <v>25</v>
@@ -1243,7 +1270,7 @@
         <v>31</v>
       </c>
       <c r="D17" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="E17" t="s">
         <v>33</v>
@@ -1260,6 +1287,12 @@
         <v>22</v>
       </c>
       <c r="K17" s="2"/>
+      <c r="L17" t="s">
+        <v>23</v>
+      </c>
+      <c r="M17" t="s">
+        <v>23</v>
+      </c>
       <c r="N17" t="s">
         <v>22</v>
       </c>
@@ -1278,7 +1311,7 @@
         <v>31</v>
       </c>
       <c r="D18" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="E18" t="s">
         <v>32</v>
@@ -1295,6 +1328,12 @@
         <v>22</v>
       </c>
       <c r="K18" s="2"/>
+      <c r="L18" t="s">
+        <v>24</v>
+      </c>
+      <c r="M18" t="s">
+        <v>24</v>
+      </c>
       <c r="N18" t="s">
         <v>22</v>
       </c>
@@ -1313,7 +1352,7 @@
         <v>31</v>
       </c>
       <c r="D19" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="E19" t="s">
         <v>20</v>
@@ -1337,10 +1376,10 @@
         <v>43897</v>
       </c>
       <c r="L19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N19" t="s">
         <v>21</v>
@@ -1360,7 +1399,7 @@
         <v>31</v>
       </c>
       <c r="D20" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="E20" t="s">
         <v>25</v>
@@ -1407,7 +1446,7 @@
         <v>31</v>
       </c>
       <c r="D21" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="E21" t="s">
         <v>33</v>
@@ -1426,6 +1465,12 @@
         <v>22</v>
       </c>
       <c r="K21" s="2"/>
+      <c r="L21" t="s">
+        <v>23</v>
+      </c>
+      <c r="M21" t="s">
+        <v>23</v>
+      </c>
       <c r="N21" t="s">
         <v>21</v>
       </c>

</xml_diff>